<commit_message>
Update analysis and readme
</commit_message>
<xml_diff>
--- a/datasets/weekly_sales_data.xlsx
+++ b/datasets/weekly_sales_data.xlsx
@@ -461,7 +461,7 @@
         <v>43485</v>
       </c>
       <c r="C4">
-        <v>13460</v>
+        <v>12595</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -470,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -521,7 +521,7 @@
         <v>43506</v>
       </c>
       <c r="C7">
-        <v>12447</v>
+        <v>13303</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -561,7 +561,7 @@
         <v>43520</v>
       </c>
       <c r="C9">
-        <v>13539</v>
+        <v>12668</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -570,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -681,7 +681,7 @@
         <v>43562</v>
       </c>
       <c r="C15">
-        <v>12500</v>
+        <v>13359</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -701,7 +701,7 @@
         <v>43569</v>
       </c>
       <c r="C16">
-        <v>12343</v>
+        <v>13192</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -721,7 +721,7 @@
         <v>43576</v>
       </c>
       <c r="C17">
-        <v>16322</v>
+        <v>17444</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -730,7 +730,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -741,7 +741,7 @@
         <v>43583</v>
       </c>
       <c r="C18">
-        <v>13275</v>
+        <v>12422</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -750,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -781,7 +781,7 @@
         <v>43597</v>
       </c>
       <c r="C20">
-        <v>12632</v>
+        <v>13500</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -790,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -801,7 +801,7 @@
         <v>43604</v>
       </c>
       <c r="C21">
-        <v>12374</v>
+        <v>13224</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -810,7 +810,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -821,7 +821,7 @@
         <v>43611</v>
       </c>
       <c r="C22">
-        <v>12692</v>
+        <v>13565</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -830,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -841,7 +841,7 @@
         <v>43618</v>
       </c>
       <c r="C23">
-        <v>12289</v>
+        <v>13134</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -881,7 +881,7 @@
         <v>43632</v>
       </c>
       <c r="C25">
-        <v>12447</v>
+        <v>13303</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -901,7 +901,7 @@
         <v>43639</v>
       </c>
       <c r="C26">
-        <v>12709</v>
+        <v>13582</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -910,7 +910,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -941,7 +941,7 @@
         <v>43653</v>
       </c>
       <c r="C28">
-        <v>12643</v>
+        <v>13512</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -950,7 +950,7 @@
         <v>350</v>
       </c>
       <c r="F28">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1021,7 +1021,7 @@
         <v>43681</v>
       </c>
       <c r="C32">
-        <v>16080</v>
+        <v>17185</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1030,7 +1030,7 @@
         <v>350</v>
       </c>
       <c r="F32">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1241,7 +1241,7 @@
         <v>43758</v>
       </c>
       <c r="C43">
-        <v>12413</v>
+        <v>13266</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1301,7 +1301,7 @@
         <v>43779</v>
       </c>
       <c r="C46">
-        <v>12650</v>
+        <v>13520</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -1310,7 +1310,7 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1321,7 +1321,7 @@
         <v>43786</v>
       </c>
       <c r="C47">
-        <v>12259</v>
+        <v>13102</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1330,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1401,7 +1401,7 @@
         <v>43814</v>
       </c>
       <c r="C51">
-        <v>12458</v>
+        <v>13314</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1410,7 +1410,7 @@
         <v>200</v>
       </c>
       <c r="F51">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1421,7 +1421,7 @@
         <v>43821</v>
       </c>
       <c r="C52">
-        <v>13402</v>
+        <v>12540</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -1430,7 +1430,7 @@
         <v>200</v>
       </c>
       <c r="F52">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="53" spans="1:6">

</xml_diff>

<commit_message>
notice mistake and fixed
</commit_message>
<xml_diff>
--- a/datasets/weekly_sales_data.xlsx
+++ b/datasets/weekly_sales_data.xlsx
@@ -461,7 +461,7 @@
         <v>43480</v>
       </c>
       <c r="C4">
-        <v>12595</v>
+        <v>13460</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -470,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -541,7 +541,7 @@
         <v>43508</v>
       </c>
       <c r="C8">
-        <v>12536</v>
+        <v>13397</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -550,7 +550,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -581,7 +581,7 @@
         <v>43522</v>
       </c>
       <c r="C10">
-        <v>12527</v>
+        <v>13388</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -601,7 +601,7 @@
         <v>43529</v>
       </c>
       <c r="C11">
-        <v>12467</v>
+        <v>13324</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -610,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -641,7 +641,7 @@
         <v>43543</v>
       </c>
       <c r="C13">
-        <v>12601</v>
+        <v>13467</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -650,7 +650,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -781,7 +781,7 @@
         <v>43592</v>
       </c>
       <c r="C20">
-        <v>12632</v>
+        <v>13500</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -790,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -841,7 +841,7 @@
         <v>43613</v>
       </c>
       <c r="C23">
-        <v>13134</v>
+        <v>12289</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -921,7 +921,7 @@
         <v>43641</v>
       </c>
       <c r="C27">
-        <v>12434</v>
+        <v>13288</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -941,7 +941,7 @@
         <v>43648</v>
       </c>
       <c r="C28">
-        <v>12643</v>
+        <v>13512</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -950,7 +950,7 @@
         <v>350</v>
       </c>
       <c r="F28">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -961,7 +961,7 @@
         <v>43655</v>
       </c>
       <c r="C29">
-        <v>12389</v>
+        <v>13240</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -970,7 +970,7 @@
         <v>350</v>
       </c>
       <c r="F29">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -981,7 +981,7 @@
         <v>43662</v>
       </c>
       <c r="C30">
-        <v>13060</v>
+        <v>12220</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -990,7 +990,7 @@
         <v>350</v>
       </c>
       <c r="F30">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1021,7 +1021,7 @@
         <v>43676</v>
       </c>
       <c r="C32">
-        <v>17185</v>
+        <v>16080</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1030,7 +1030,7 @@
         <v>350</v>
       </c>
       <c r="F32">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1041,7 +1041,7 @@
         <v>43683</v>
       </c>
       <c r="C33">
-        <v>13163</v>
+        <v>12316</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1050,7 +1050,7 @@
         <v>350</v>
       </c>
       <c r="F33">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1081,7 +1081,7 @@
         <v>43697</v>
       </c>
       <c r="C35">
-        <v>13299</v>
+        <v>12444</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1090,7 +1090,7 @@
         <v>350</v>
       </c>
       <c r="F35">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1101,7 +1101,7 @@
         <v>43704</v>
       </c>
       <c r="C36">
-        <v>17448</v>
+        <v>16326</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1110,7 +1110,7 @@
         <v>350</v>
       </c>
       <c r="F36">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1121,7 +1121,7 @@
         <v>43711</v>
       </c>
       <c r="C37">
-        <v>12313</v>
+        <v>13160</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1130,7 +1130,7 @@
         <v>350</v>
       </c>
       <c r="F37">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1181,7 +1181,7 @@
         <v>43732</v>
       </c>
       <c r="C40">
-        <v>12506</v>
+        <v>13365</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1201,7 +1201,7 @@
         <v>43739</v>
       </c>
       <c r="C41">
-        <v>13406</v>
+        <v>12544</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1210,7 +1210,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1221,7 +1221,7 @@
         <v>43746</v>
       </c>
       <c r="C42">
-        <v>12551</v>
+        <v>13414</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1230,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1241,7 +1241,7 @@
         <v>43753</v>
       </c>
       <c r="C43">
-        <v>12413</v>
+        <v>13266</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1301,7 +1301,7 @@
         <v>43774</v>
       </c>
       <c r="C46">
-        <v>13520</v>
+        <v>12650</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -1310,7 +1310,7 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1341,7 +1341,7 @@
         <v>43788</v>
       </c>
       <c r="C48">
-        <v>17151</v>
+        <v>16049</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1350,7 +1350,7 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1361,7 +1361,7 @@
         <v>43795</v>
       </c>
       <c r="C49">
-        <v>13595</v>
+        <v>12721</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1401,7 +1401,7 @@
         <v>43809</v>
       </c>
       <c r="C51">
-        <v>12458</v>
+        <v>13314</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1410,7 +1410,7 @@
         <v>200</v>
       </c>
       <c r="F51">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1441,7 +1441,7 @@
         <v>43823</v>
       </c>
       <c r="C53">
-        <v>13330</v>
+        <v>12473</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -1450,7 +1450,7 @@
         <v>200</v>
       </c>
       <c r="F53">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add simulation data to repo
</commit_message>
<xml_diff>
--- a/datasets/weekly_sales_data.xlsx
+++ b/datasets/weekly_sales_data.xlsx
@@ -421,7 +421,7 @@
         <v>43466</v>
       </c>
       <c r="C2">
-        <v>13460</v>
+        <v>12595</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -430,7 +430,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -461,7 +461,7 @@
         <v>43480</v>
       </c>
       <c r="C4">
-        <v>13460</v>
+        <v>12595</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -470,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -501,7 +501,7 @@
         <v>43494</v>
       </c>
       <c r="C6">
-        <v>13668</v>
+        <v>12789</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -510,7 +510,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -521,7 +521,7 @@
         <v>43501</v>
       </c>
       <c r="C7">
-        <v>12447</v>
+        <v>13303</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -541,7 +541,7 @@
         <v>43508</v>
       </c>
       <c r="C8">
-        <v>13397</v>
+        <v>12536</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -550,7 +550,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -561,7 +561,7 @@
         <v>43515</v>
       </c>
       <c r="C9">
-        <v>13539</v>
+        <v>12668</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -570,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -581,7 +581,7 @@
         <v>43522</v>
       </c>
       <c r="C10">
-        <v>13388</v>
+        <v>12527</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -621,7 +621,7 @@
         <v>43536</v>
       </c>
       <c r="C12">
-        <v>12346</v>
+        <v>13195</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -661,7 +661,7 @@
         <v>43550</v>
       </c>
       <c r="C14">
-        <v>13197</v>
+        <v>12348</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -670,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -681,7 +681,7 @@
         <v>43557</v>
       </c>
       <c r="C15">
-        <v>13359</v>
+        <v>12500</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -721,7 +721,7 @@
         <v>43571</v>
       </c>
       <c r="C17">
-        <v>16322</v>
+        <v>17444</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -730,7 +730,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -741,7 +741,7 @@
         <v>43578</v>
       </c>
       <c r="C18">
-        <v>12422</v>
+        <v>13275</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -750,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -761,7 +761,7 @@
         <v>43585</v>
       </c>
       <c r="C19">
-        <v>13479</v>
+        <v>12613</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -801,7 +801,7 @@
         <v>43599</v>
       </c>
       <c r="C21">
-        <v>13224</v>
+        <v>12374</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -810,7 +810,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -841,7 +841,7 @@
         <v>43613</v>
       </c>
       <c r="C23">
-        <v>12289</v>
+        <v>13134</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -861,7 +861,7 @@
         <v>43620</v>
       </c>
       <c r="C24">
-        <v>12495</v>
+        <v>13354</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -870,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -881,7 +881,7 @@
         <v>43627</v>
       </c>
       <c r="C25">
-        <v>13303</v>
+        <v>12447</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -921,7 +921,7 @@
         <v>43641</v>
       </c>
       <c r="C27">
-        <v>13288</v>
+        <v>12434</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -961,7 +961,7 @@
         <v>43655</v>
       </c>
       <c r="C29">
-        <v>13240</v>
+        <v>12389</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -970,7 +970,7 @@
         <v>350</v>
       </c>
       <c r="F29">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -981,7 +981,7 @@
         <v>43662</v>
       </c>
       <c r="C30">
-        <v>12220</v>
+        <v>13060</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -990,7 +990,7 @@
         <v>350</v>
       </c>
       <c r="F30">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1081,7 +1081,7 @@
         <v>43697</v>
       </c>
       <c r="C35">
-        <v>12444</v>
+        <v>13299</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1090,7 +1090,7 @@
         <v>350</v>
       </c>
       <c r="F35">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1101,7 +1101,7 @@
         <v>43704</v>
       </c>
       <c r="C36">
-        <v>16326</v>
+        <v>17448</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1110,7 +1110,7 @@
         <v>350</v>
       </c>
       <c r="F36">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1161,7 +1161,7 @@
         <v>43725</v>
       </c>
       <c r="C39">
-        <v>17093</v>
+        <v>15994</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1170,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1181,7 +1181,7 @@
         <v>43732</v>
       </c>
       <c r="C40">
-        <v>13365</v>
+        <v>12506</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1201,7 +1201,7 @@
         <v>43739</v>
       </c>
       <c r="C41">
-        <v>12544</v>
+        <v>13406</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1210,7 +1210,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1221,7 +1221,7 @@
         <v>43746</v>
       </c>
       <c r="C42">
-        <v>13414</v>
+        <v>12551</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1230,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1241,7 +1241,7 @@
         <v>43753</v>
       </c>
       <c r="C43">
-        <v>13266</v>
+        <v>12413</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1261,7 +1261,7 @@
         <v>43760</v>
       </c>
       <c r="C44">
-        <v>12559</v>
+        <v>13422</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -1270,7 +1270,7 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1321,7 +1321,7 @@
         <v>43781</v>
       </c>
       <c r="C47">
-        <v>13102</v>
+        <v>12259</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1330,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1401,7 +1401,7 @@
         <v>43809</v>
       </c>
       <c r="C51">
-        <v>13314</v>
+        <v>12458</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1410,7 +1410,7 @@
         <v>200</v>
       </c>
       <c r="F51">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1441,7 +1441,7 @@
         <v>43823</v>
       </c>
       <c r="C53">
-        <v>12473</v>
+        <v>13330</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -1450,7 +1450,7 @@
         <v>200</v>
       </c>
       <c r="F53">
-        <v>4.5</v>
+        <v>4.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>